<commit_message>
update nomenclature - FEAR to Schedonorus arundinaceus
</commit_message>
<xml_diff>
--- a/d1979_formatted-METADATA.xlsx
+++ b/d1979_formatted-METADATA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/stefanie_lane_ubc_ca/Documents/Documents/Dissertation/CommunityStability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\CommunityStability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{2E6D9C51-2000-464F-879B-2B3334A54051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{784095EE-20D3-400F-9B24-3FCB5A3F443B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{2E6D9C51-2000-464F-879B-2B3334A54051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E01CF885-ED20-4868-83EF-08C4D91D428B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,16 +569,16 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
@@ -687,17 +687,17 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -772,17 +772,33 @@
       <c r="H14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -1011,22 +1027,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78641E9-6B89-49F8-A64B-E70C791B6886}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4901A729-BF60-4E35-96E4-F33CC664023D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C45E3C36-D906-456C-888F-720E462F2C07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1043,29 +1069,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4901A729-BF60-4E35-96E4-F33CC664023D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78641E9-6B89-49F8-A64B-E70C791B6886}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>